<commit_message>
build: 1.01 add patient info, email, phone number and corr. validation, add ability to continue survey from loaded responses
</commit_message>
<xml_diff>
--- a/Questions/Questions.xlsx
+++ b/Questions/Questions.xlsx
@@ -20,7 +20,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="291">
+  <si>
+    <t xml:space="preserve">Question ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Questions</t>
+  </si>
   <si>
     <t xml:space="preserve">Among my greatest strengths is the depth of  my feelings/ Among my greatest strengths is the sharpness of my mind</t>
   </si>
@@ -1203,10 +1209,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:FI1048576"/>
+  <dimension ref="A1:FI413"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.41796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1218,1327 +1224,1287 @@
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="n">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>1</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>0</v>
       </c>
     </row>
     <row r="2" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>2</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="3" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>3</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="4" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>4</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="5" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>5</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="6" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>6</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="7" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>7</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="8" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="9" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="10" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="11" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="12" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>12</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="13" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="14" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="15" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="16" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="17" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="18" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="19" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>19</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="20" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="21" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="22" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="23" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="24" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="25" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="26" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="27" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="3" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="28" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B28" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F28" s="4"/>
     </row>
     <row r="29" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="3" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B29" s="3" t="s">
-        <v>28</v>
-      </c>
+      <c r="F29" s="4"/>
     </row>
     <row r="30" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="31" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="32" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="3" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B32" s="3" t="s">
-        <v>31</v>
-      </c>
     </row>
     <row r="33" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="4" t="n">
+      <c r="A33" s="3" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B33" s="3" t="s">
-        <v>32</v>
-      </c>
     </row>
     <row r="34" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="3" t="n">
+      <c r="A34" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="35" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="3" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="36" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="3" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" s="3" t="s">
         <v>36</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="37" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="3" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="38" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="3" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B38" s="3" t="s">
-        <v>37</v>
-      </c>
     </row>
     <row r="39" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="4" t="n">
+      <c r="A39" s="3" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B39" s="3" t="s">
-        <v>38</v>
-      </c>
     </row>
     <row r="40" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="3" t="n">
+      <c r="A40" s="4" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" s="3" t="s">
         <v>40</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="41" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" s="3" t="s">
         <v>41</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="42" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="3" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" s="3" t="s">
         <v>42</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="43" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="3" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" s="3" t="s">
         <v>43</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="44" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="3" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" s="3" t="s">
         <v>44</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="45" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="3" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" s="3" t="s">
         <v>45</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="46" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="3" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" s="3" t="s">
         <v>46</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="47" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="3" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" s="3" t="s">
         <v>47</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="48" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="3" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" s="3" t="s">
         <v>48</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="49" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="3" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" s="3" t="s">
         <v>49</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="50" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="3" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" s="3" t="s">
         <v>50</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="51" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="3" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" s="3" t="s">
         <v>51</v>
-      </c>
-      <c r="B51" s="3" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="52" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="3" t="n">
+        <v>51</v>
+      </c>
+      <c r="B52" s="3" t="s">
         <v>52</v>
-      </c>
-      <c r="B52" s="3" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="53" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="3" t="n">
+        <v>52</v>
+      </c>
+      <c r="B53" s="3" t="s">
         <v>53</v>
-      </c>
-      <c r="B53" s="3" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="54" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="3" t="n">
+        <v>53</v>
+      </c>
+      <c r="B54" s="3" t="s">
         <v>54</v>
-      </c>
-      <c r="B54" s="3" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="55" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="3" t="n">
+        <v>54</v>
+      </c>
+      <c r="B55" s="3" t="s">
         <v>55</v>
-      </c>
-      <c r="B55" s="3" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="56" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="3" t="n">
+        <v>55</v>
+      </c>
+      <c r="B56" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="B56" s="3" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="57" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="3" t="n">
+        <v>56</v>
+      </c>
+      <c r="B57" s="3" t="s">
         <v>57</v>
-      </c>
-      <c r="B57" s="3" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="58" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="3" t="n">
+        <v>57</v>
+      </c>
+      <c r="B58" s="3" t="s">
         <v>58</v>
-      </c>
-      <c r="B58" s="3" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="59" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="3" t="n">
+        <v>58</v>
+      </c>
+      <c r="B59" s="3" t="s">
         <v>59</v>
-      </c>
-      <c r="B59" s="3" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="60" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="3" t="n">
+        <v>59</v>
+      </c>
+      <c r="B60" s="3" t="s">
         <v>60</v>
-      </c>
-      <c r="B60" s="3" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="61" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="3" t="n">
+        <v>60</v>
+      </c>
+      <c r="B61" s="3" t="s">
         <v>61</v>
-      </c>
-      <c r="B61" s="3" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="62" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="3" t="n">
+        <v>61</v>
+      </c>
+      <c r="B62" s="3" t="s">
         <v>62</v>
-      </c>
-      <c r="B62" s="3" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="63" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="3" t="n">
+        <v>62</v>
+      </c>
+      <c r="B63" s="3" t="s">
         <v>63</v>
-      </c>
-      <c r="B63" s="3" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="64" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="3" t="n">
+        <v>63</v>
+      </c>
+      <c r="B64" s="3" t="s">
         <v>64</v>
-      </c>
-      <c r="B64" s="3" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="65" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="3" t="n">
+        <v>64</v>
+      </c>
+      <c r="B65" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B65" s="3" t="s">
-        <v>64</v>
-      </c>
     </row>
     <row r="66" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A66" s="4" t="n">
+      <c r="A66" s="3" t="n">
+        <v>65</v>
+      </c>
+      <c r="B66" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B66" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="I66" s="4"/>
-      <c r="J66" s="4"/>
     </row>
     <row r="67" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A67" s="3" t="n">
+      <c r="A67" s="4" t="n">
+        <v>66</v>
+      </c>
+      <c r="B67" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B67" s="3" t="s">
-        <v>66</v>
-      </c>
+      <c r="I67" s="4"/>
+      <c r="J67" s="4"/>
     </row>
     <row r="68" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="3" t="n">
+        <v>67</v>
+      </c>
+      <c r="B68" s="3" t="s">
         <v>68</v>
-      </c>
-      <c r="B68" s="3" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="69" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="3" t="n">
+        <v>68</v>
+      </c>
+      <c r="B69" s="3" t="s">
         <v>69</v>
-      </c>
-      <c r="B69" s="3" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="70" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="3" t="n">
+        <v>69</v>
+      </c>
+      <c r="B70" s="3" t="s">
         <v>70</v>
-      </c>
-      <c r="B70" s="3" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="71" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="3" t="n">
+        <v>70</v>
+      </c>
+      <c r="B71" s="3" t="s">
         <v>71</v>
-      </c>
-      <c r="B71" s="3" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="72" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="3" t="n">
+        <v>71</v>
+      </c>
+      <c r="B72" s="3" t="s">
         <v>72</v>
-      </c>
-      <c r="B72" s="3" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="73" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="3" t="n">
+        <v>72</v>
+      </c>
+      <c r="B73" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="B73" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="P73" s="4"/>
     </row>
     <row r="74" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="3" t="n">
+        <v>73</v>
+      </c>
+      <c r="B74" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="B74" s="3" t="s">
-        <v>73</v>
-      </c>
+      <c r="P74" s="4"/>
     </row>
     <row r="75" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="3" t="n">
+        <v>74</v>
+      </c>
+      <c r="B75" s="3" t="s">
         <v>75</v>
-      </c>
-      <c r="B75" s="3" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="76" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="3" t="n">
+        <v>75</v>
+      </c>
+      <c r="B76" s="3" t="s">
         <v>76</v>
-      </c>
-      <c r="B76" s="3" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="77" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="3" t="n">
+        <v>76</v>
+      </c>
+      <c r="B77" s="3" t="s">
         <v>77</v>
-      </c>
-      <c r="B77" s="3" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="78" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="3" t="n">
+        <v>77</v>
+      </c>
+      <c r="B78" s="3" t="s">
         <v>78</v>
-      </c>
-      <c r="B78" s="3" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="79" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="3" t="n">
+        <v>78</v>
+      </c>
+      <c r="B79" s="3" t="s">
         <v>79</v>
-      </c>
-      <c r="B79" s="3" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="80" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A80" s="3" t="n">
+        <v>79</v>
+      </c>
+      <c r="B80" s="3" t="s">
         <v>80</v>
-      </c>
-      <c r="B80" s="3" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="81" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="3" t="n">
+        <v>80</v>
+      </c>
+      <c r="B81" s="3" t="s">
         <v>81</v>
-      </c>
-      <c r="B81" s="3" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="82" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="3" t="n">
+        <v>81</v>
+      </c>
+      <c r="B82" s="3" t="s">
         <v>82</v>
-      </c>
-      <c r="B82" s="3" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="83" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A83" s="3" t="n">
+        <v>82</v>
+      </c>
+      <c r="B83" s="3" t="s">
         <v>83</v>
-      </c>
-      <c r="B83" s="3" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="84" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="3" t="n">
+        <v>83</v>
+      </c>
+      <c r="B84" s="3" t="s">
         <v>84</v>
-      </c>
-      <c r="B84" s="3" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="85" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A85" s="3" t="n">
+        <v>84</v>
+      </c>
+      <c r="B85" s="3" t="s">
         <v>85</v>
-      </c>
-      <c r="B85" s="3" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="86" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A86" s="3" t="n">
+        <v>85</v>
+      </c>
+      <c r="B86" s="3" t="s">
         <v>86</v>
-      </c>
-      <c r="B86" s="3" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="87" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A87" s="3" t="n">
+        <v>86</v>
+      </c>
+      <c r="B87" s="3" t="s">
         <v>87</v>
-      </c>
-      <c r="B87" s="3" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="88" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A88" s="3" t="n">
+        <v>87</v>
+      </c>
+      <c r="B88" s="3" t="s">
         <v>88</v>
-      </c>
-      <c r="B88" s="3" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="89" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A89" s="3" t="n">
+        <v>88</v>
+      </c>
+      <c r="B89" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="B89" s="3" t="s">
-        <v>88</v>
-      </c>
     </row>
     <row r="90" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A90" s="4" t="n">
+      <c r="A90" s="3" t="n">
+        <v>89</v>
+      </c>
+      <c r="B90" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="B90" s="3" t="s">
-        <v>89</v>
-      </c>
     </row>
     <row r="91" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A91" s="3" t="n">
+      <c r="A91" s="4" t="n">
+        <v>90</v>
+      </c>
+      <c r="B91" s="3" t="s">
         <v>91</v>
-      </c>
-      <c r="B91" s="3" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="92" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A92" s="3" t="n">
+        <v>91</v>
+      </c>
+      <c r="B92" s="3" t="s">
         <v>92</v>
-      </c>
-      <c r="B92" s="3" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="93" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A93" s="3" t="n">
+        <v>92</v>
+      </c>
+      <c r="B93" s="3" t="s">
         <v>93</v>
-      </c>
-      <c r="B93" s="3" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="94" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A94" s="3" t="n">
+        <v>93</v>
+      </c>
+      <c r="B94" s="3" t="s">
         <v>94</v>
-      </c>
-      <c r="B94" s="3" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="95" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A95" s="3" t="n">
+        <v>94</v>
+      </c>
+      <c r="B95" s="3" t="s">
         <v>95</v>
-      </c>
-      <c r="B95" s="3" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="96" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A96" s="3" t="n">
+        <v>95</v>
+      </c>
+      <c r="B96" s="3" t="s">
         <v>96</v>
-      </c>
-      <c r="B96" s="3" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="97" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A97" s="3" t="n">
+        <v>96</v>
+      </c>
+      <c r="B97" s="3" t="s">
         <v>97</v>
-      </c>
-      <c r="B97" s="3" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="98" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A98" s="3" t="n">
+        <v>97</v>
+      </c>
+      <c r="B98" s="3" t="s">
         <v>98</v>
-      </c>
-      <c r="B98" s="3" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="99" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A99" s="3" t="n">
+        <v>98</v>
+      </c>
+      <c r="B99" s="3" t="s">
         <v>99</v>
-      </c>
-      <c r="B99" s="3" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="100" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A100" s="3" t="n">
+        <v>99</v>
+      </c>
+      <c r="B100" s="3" t="s">
         <v>100</v>
-      </c>
-      <c r="B100" s="3" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="101" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A101" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="B101" s="3" t="s">
         <v>101</v>
-      </c>
-      <c r="B101" s="3" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="102" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A102" s="3" t="n">
+        <v>101</v>
+      </c>
+      <c r="B102" s="3" t="s">
         <v>102</v>
-      </c>
-      <c r="B102" s="3" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="103" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A103" s="3" t="n">
+        <v>102</v>
+      </c>
+      <c r="B103" s="3" t="s">
         <v>103</v>
-      </c>
-      <c r="B103" s="3" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="104" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A104" s="3" t="n">
+        <v>103</v>
+      </c>
+      <c r="B104" s="3" t="s">
         <v>104</v>
-      </c>
-      <c r="B104" s="3" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="105" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A105" s="3" t="n">
+        <v>104</v>
+      </c>
+      <c r="B105" s="3" t="s">
         <v>105</v>
-      </c>
-      <c r="B105" s="3" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="106" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A106" s="3" t="n">
+        <v>105</v>
+      </c>
+      <c r="B106" s="3" t="s">
         <v>106</v>
-      </c>
-      <c r="B106" s="3" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="107" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A107" s="3" t="n">
+        <v>106</v>
+      </c>
+      <c r="B107" s="3" t="s">
         <v>107</v>
-      </c>
-      <c r="B107" s="3" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="108" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A108" s="3" t="n">
+        <v>107</v>
+      </c>
+      <c r="B108" s="3" t="s">
         <v>108</v>
-      </c>
-      <c r="B108" s="3" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="109" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A109" s="3" t="n">
+        <v>108</v>
+      </c>
+      <c r="B109" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="B109" s="3" t="s">
-        <v>108</v>
-      </c>
     </row>
     <row r="110" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A110" s="4" t="n">
+      <c r="A110" s="3" t="n">
+        <v>109</v>
+      </c>
+      <c r="B110" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="B110" s="3" t="s">
-        <v>109</v>
-      </c>
     </row>
     <row r="111" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A111" s="3" t="n">
+      <c r="A111" s="4" t="n">
+        <v>110</v>
+      </c>
+      <c r="B111" s="3" t="s">
         <v>111</v>
-      </c>
-      <c r="B111" s="3" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="112" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A112" s="3" t="n">
+        <v>111</v>
+      </c>
+      <c r="B112" s="3" t="s">
         <v>112</v>
-      </c>
-      <c r="B112" s="3" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="113" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A113" s="3" t="n">
+        <v>112</v>
+      </c>
+      <c r="B113" s="3" t="s">
         <v>113</v>
-      </c>
-      <c r="B113" s="3" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="114" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A114" s="3" t="n">
+        <v>113</v>
+      </c>
+      <c r="B114" s="3" t="s">
         <v>114</v>
-      </c>
-      <c r="B114" s="3" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="115" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A115" s="3" t="n">
+        <v>114</v>
+      </c>
+      <c r="B115" s="3" t="s">
         <v>115</v>
-      </c>
-      <c r="B115" s="3" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="116" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A116" s="3" t="n">
+        <v>115</v>
+      </c>
+      <c r="B116" s="3" t="s">
         <v>116</v>
-      </c>
-      <c r="B116" s="3" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="117" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A117" s="3" t="n">
+        <v>116</v>
+      </c>
+      <c r="B117" s="3" t="s">
         <v>117</v>
-      </c>
-      <c r="B117" s="3" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="118" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A118" s="3" t="n">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="BW118" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="CD118" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="DD118" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="DK118" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="FB118" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="FI118" s="3" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="119" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A119" s="3" t="n">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B119" s="3" t="s">
         <v>119</v>
       </c>
+      <c r="BW119" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="CD119" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="DD119" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="DK119" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="FB119" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="FI119" s="3" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="120" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A120" s="3" t="n">
+        <v>119</v>
+      </c>
+      <c r="B120" s="3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="121" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A121" s="3" t="n">
         <v>120</v>
       </c>
-      <c r="B120" s="3" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="121" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A121" s="4" t="n">
+      <c r="B121" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="122" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A122" s="4" t="n">
         <v>121</v>
       </c>
-      <c r="B121" s="3" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="122" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A122" s="3" t="n">
-        <v>122</v>
-      </c>
       <c r="B122" s="3" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="123" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A123" s="3" t="n">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="124" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A124" s="3" t="n">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="125" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A125" s="3" t="n">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="126" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A126" s="3" t="n">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="127" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A127" s="3" t="n">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="128" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A128" s="3" t="n">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="129" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A129" s="3" t="n">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B129" s="3" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="130" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A130" s="3" t="n">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="N130" s="4"/>
+        <v>131</v>
+      </c>
     </row>
     <row r="131" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A131" s="3" t="n">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B131" s="3" t="s">
-        <v>131</v>
-      </c>
+        <v>132</v>
+      </c>
+      <c r="N131" s="4"/>
     </row>
     <row r="132" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A132" s="3" t="n">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B132" s="3" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="133" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A133" s="3" t="n">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="134" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A134" s="3" t="n">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B134" s="3" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="135" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A135" s="3" t="n">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="136" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A136" s="3" t="n">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="137" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A137" s="3" t="n">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="138" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A138" s="3" t="n">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="139" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A139" s="3" t="n">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B139" s="3" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="140" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A140" s="3" t="n">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B140" s="3" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="141" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A141" s="3" t="n">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B141" s="3" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="142" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A142" s="3" t="n">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B142" s="3" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="143" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A143" s="3" t="n">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B143" s="3" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="144" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A144" s="3" t="n">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B144" s="3" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="145" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A145" s="3" t="n">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="146" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A146" s="3" t="n">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="147" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A147" s="3" t="n">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B147" s="3" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="148" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A148" s="3" t="n">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B148" s="3" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="149" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A149" s="3" t="n">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B149" s="3" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="150" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A150" s="3" t="n">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B150" s="3" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="151" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A151" s="3" t="n">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B151" s="3" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="152" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A152" s="3" t="n">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B152" s="3" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="153" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A153" s="3" t="n">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B153" s="3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="154" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A154" s="3" t="n">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B154" s="3" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="155" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A155" s="3" t="n">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B155" s="3" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="156" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A156" s="3" t="n">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B156" s="3" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="157" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A157" s="3" t="n">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B157" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="DK157" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="DL157" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="DM157" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="DN157" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="DO157" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="DP157" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="DQ157" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="DY157" s="3" t="n">
-        <f aca="false">DY156+1</f>
-        <v>1</v>
-      </c>
-      <c r="DZ157" s="3" t="s">
         <v>158</v>
-      </c>
-      <c r="EY157" s="3" t="e">
-        <f aca="false">VLOOKUP(A3459,$DY$3:$DZ$300,2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="EZ157" s="3" t="n">
-        <f aca="false">DY157</f>
-        <v>1</v>
-      </c>
-      <c r="FA157" s="3" t="n">
-        <f aca="false">A3459</f>
-        <v>0</v>
       </c>
     </row>
     <row r="158" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A158" s="3" t="n">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B158" s="3" t="s">
         <v>159</v>
@@ -2566,18 +2532,18 @@
       </c>
       <c r="DY158" s="3" t="n">
         <f aca="false">DY157+1</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="DZ158" s="3" t="s">
         <v>160</v>
       </c>
       <c r="EY158" s="3" t="e">
-        <f aca="false">VLOOKUP(A3460,$DY$3:$DZ$300,2)</f>
+        <f aca="false">VLOOKUP(A3460,$DY$4:$DZ$301,2)</f>
         <v>#N/A</v>
       </c>
       <c r="EZ158" s="3" t="n">
         <f aca="false">DY158</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="FA158" s="3" t="n">
         <f aca="false">A3460</f>
@@ -2586,7 +2552,7 @@
     </row>
     <row r="159" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A159" s="3" t="n">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B159" s="3" t="s">
         <v>161</v>
@@ -2614,18 +2580,18 @@
       </c>
       <c r="DY159" s="3" t="n">
         <f aca="false">DY158+1</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="DZ159" s="3" t="s">
         <v>162</v>
       </c>
       <c r="EY159" s="3" t="e">
-        <f aca="false">VLOOKUP(A3461,$DY$3:$DZ$300,2)</f>
+        <f aca="false">VLOOKUP(A3461,$DY$4:$DZ$301,2)</f>
         <v>#N/A</v>
       </c>
       <c r="EZ159" s="3" t="n">
         <f aca="false">DY159</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="FA159" s="3" t="n">
         <f aca="false">A3461</f>
@@ -2634,1024 +2600,1069 @@
     </row>
     <row r="160" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A160" s="3" t="n">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B160" s="3" t="s">
         <v>163</v>
       </c>
+      <c r="DK160" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="DL160" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="DM160" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="DN160" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="DO160" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="DP160" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="DQ160" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="DY160" s="3" t="n">
+        <f aca="false">DY159+1</f>
+        <v>3</v>
+      </c>
+      <c r="DZ160" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="EY160" s="3" t="e">
+        <f aca="false">VLOOKUP(A3462,$DY$4:$DZ$301,2)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="EZ160" s="3" t="n">
+        <f aca="false">DY160</f>
+        <v>3</v>
+      </c>
+      <c r="FA160" s="3" t="n">
+        <f aca="false">A3462</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="161" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A161" s="3" t="n">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B161" s="3" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="162" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A162" s="3" t="n">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B162" s="3" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="163" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A163" s="3" t="n">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B163" s="3" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="164" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A164" s="3" t="n">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B164" s="3" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="165" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A165" s="3" t="n">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B165" s="3" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="166" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A166" s="3" t="n">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B166" s="3" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="167" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A167" s="3" t="n">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B167" s="3" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="168" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A168" s="3" t="n">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B168" s="3" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="169" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A169" s="3" t="n">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B169" s="3" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="170" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A170" s="3" t="n">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B170" s="3" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="171" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A171" s="3" t="n">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B171" s="3" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="172" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A172" s="3" t="n">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B172" s="3" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="173" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A173" s="3" t="n">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B173" s="3" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="174" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A174" s="3" t="n">
+        <v>173</v>
+      </c>
+      <c r="B174" s="3" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="175" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A175" s="3" t="n">
         <v>174</v>
       </c>
-      <c r="B174" s="3" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="175" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A175" s="4" t="n">
+      <c r="B175" s="3" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="176" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A176" s="4" t="n">
         <v>175</v>
       </c>
-      <c r="B175" s="3" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="176" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A176" s="3" t="n">
-        <v>176</v>
-      </c>
       <c r="B176" s="3" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="177" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A177" s="3" t="n">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B177" s="3" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="178" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A178" s="3" t="n">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B178" s="3" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="179" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A179" s="3" t="n">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B179" s="3" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="180" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A180" s="3" t="n">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B180" s="3" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="181" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A181" s="3" t="n">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B181" s="3" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="182" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A182" s="3" t="n">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B182" s="3" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="183" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A183" s="3" t="n">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B183" s="3" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="184" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A184" s="3" t="n">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B184" s="3" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="185" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A185" s="3" t="n">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B185" s="3" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="186" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A186" s="3" t="n">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B186" s="3" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="187" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A187" s="3" t="n">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B187" s="3" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="188" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A188" s="3" t="n">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B188" s="3" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="189" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A189" s="3" t="n">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B189" s="3" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="190" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A190" s="3" t="n">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B190" s="3" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="191" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A191" s="3" t="n">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B191" s="3" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="192" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A192" s="3" t="n">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B192" s="3" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="193" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A193" s="3" t="n">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B193" s="3" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="194" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A194" s="3" t="n">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B194" s="3" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="195" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A195" s="3" t="n">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B195" s="3" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="196" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A196" s="3" t="n">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B196" s="3" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="197" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A197" s="3" t="n">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B197" s="3" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="198" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A198" s="3" t="n">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B198" s="3" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="199" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A199" s="3" t="n">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B199" s="3" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="200" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A200" s="3" t="n">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B200" s="3" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="201" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A201" s="3" t="n">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B201" s="3" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="202" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A202" s="3" t="n">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B202" s="3" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="203" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A203" s="3" t="n">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B203" s="3" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="204" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A204" s="3" t="n">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B204" s="3" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="205" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A205" s="3" t="n">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B205" s="3" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="206" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A206" s="3" t="n">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B206" s="3" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="207" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A207" s="3" t="n">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B207" s="3" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="208" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A208" s="3" t="n">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B208" s="3" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="209" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A209" s="3" t="n">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B209" s="3" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="210" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A210" s="3" t="n">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B210" s="3" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="211" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A211" s="3" t="n">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B211" s="3" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="212" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A212" s="3" t="n">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B212" s="3" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="213" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A213" s="3" t="n">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B213" s="3" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="214" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A214" s="3" t="n">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B214" s="3" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="215" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A215" s="3" t="n">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B215" s="3" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="216" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A216" s="3" t="n">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B216" s="3" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="217" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A217" s="3" t="n">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B217" s="3" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="218" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A218" s="3" t="n">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B218" s="3" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="219" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A219" s="3" t="n">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B219" s="3" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="220" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A220" s="3" t="n">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B220" s="3" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="221" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A221" s="3" t="n">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B221" s="3" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="222" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A222" s="3" t="n">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B222" s="3" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="223" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A223" s="3" t="n">
+        <v>222</v>
+      </c>
+      <c r="B223" s="3" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="224" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A224" s="3" t="n">
         <v>223</v>
       </c>
-      <c r="B223" s="3" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="224" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A224" s="4" t="n">
+      <c r="B224" s="3" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="225" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A225" s="4" t="n">
         <v>224</v>
       </c>
-      <c r="B224" s="3" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="225" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A225" s="3" t="n">
-        <v>225</v>
-      </c>
       <c r="B225" s="3" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="226" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A226" s="3" t="n">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B226" s="3" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="227" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A227" s="3" t="n">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B227" s="3" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="228" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A228" s="3" t="n">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B228" s="3" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="229" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A229" s="3" t="n">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B229" s="3" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="230" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A230" s="3" t="n">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B230" s="3" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="231" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A231" s="3" t="n">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B231" s="3" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="232" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A232" s="3" t="n">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B232" s="3" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="233" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A233" s="3" t="n">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B233" s="3" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="234" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A234" s="3" t="n">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B234" s="3" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="235" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A235" s="3" t="n">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B235" s="3" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="236" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A236" s="3" t="n">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B236" s="3" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row r="237" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A237" s="3" t="n">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B237" s="3" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="238" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A238" s="3" t="n">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B238" s="3" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="239" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A239" s="3" t="n">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B239" s="3" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="240" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A240" s="3" t="n">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B240" s="3" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="241" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A241" s="3" t="n">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B241" s="3" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="242" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A242" s="3" t="n">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B242" s="3" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="243" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A243" s="3" t="n">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B243" s="3" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="244" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A244" s="3" t="n">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B244" s="3" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="245" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A245" s="3" t="n">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B245" s="3" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="246" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A246" s="3" t="n">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B246" s="3" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="247" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A247" s="3" t="n">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B247" s="3" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="248" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A248" s="3" t="n">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B248" s="3" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="249" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A249" s="3" t="n">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B249" s="3" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="250" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A250" s="3" t="n">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B250" s="3" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="251" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A251" s="3" t="n">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B251" s="3" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="252" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A252" s="3" t="n">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B252" s="3" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="253" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A253" s="3" t="n">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B253" s="3" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="254" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A254" s="3" t="n">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B254" s="3" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="255" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A255" s="3" t="n">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B255" s="3" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="256" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A256" s="3" t="n">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B256" s="3" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="257" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A257" s="3" t="n">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B257" s="3" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="258" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A258" s="3" t="n">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B258" s="3" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="259" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A259" s="3" t="n">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B259" s="3" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="260" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A260" s="3" t="n">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B260" s="3" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="261" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A261" s="3" t="n">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B261" s="3" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="262" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A262" s="3" t="n">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B262" s="3" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="263" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A263" s="3" t="n">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B263" s="3" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="264" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A264" s="3" t="n">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B264" s="3" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="265" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A265" s="3" t="n">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B265" s="3" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="266" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A266" s="3" t="n">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B266" s="3" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="267" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A267" s="3" t="n">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B267" s="3" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="268" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A268" s="3" t="n">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B268" s="3" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="269" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A269" s="3" t="n">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B269" s="3" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="270" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A270" s="3" t="n">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B270" s="3" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="271" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A271" s="3" t="n">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B271" s="3" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="272" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A272" s="3" t="n">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B272" s="3" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="273" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A273" s="3" t="n">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B273" s="3" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="274" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A274" s="3" t="n">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B274" s="3" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="275" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A275" s="3" t="n">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B275" s="3" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="276" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A276" s="3" t="n">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B276" s="3" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="277" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A277" s="3" t="n">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B277" s="3" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="278" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A278" s="3" t="n">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B278" s="3" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="279" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A279" s="3" t="n">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B279" s="3" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="280" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A280" s="3" t="n">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B280" s="3" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="281" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A281" s="3" t="n">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B281" s="3" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="282" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A282" s="3" t="n">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B282" s="3" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="283" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A283" s="3" t="n">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B283" s="3" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="284" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A284" s="3" t="n">
+        <v>283</v>
+      </c>
+      <c r="B284" s="3" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="285" s="3" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A285" s="3" t="n">
         <v>284</v>
       </c>
-      <c r="B284" s="3" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="291" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D291" s="5"/>
-      <c r="G291" s="5"/>
-      <c r="T291" s="2"/>
+      <c r="B285" s="3" t="s">
+        <v>289</v>
+      </c>
     </row>
     <row r="292" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D292" s="5"/>
+      <c r="G292" s="5"/>
       <c r="T292" s="2"/>
     </row>
     <row r="293" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D293" s="5"/>
       <c r="T293" s="2"/>
     </row>
     <row r="294" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="T294" s="2"/>
     </row>
     <row r="295" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D295" s="5"/>
       <c r="T295" s="2"/>
     </row>
     <row r="296" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D296" s="5"/>
       <c r="T296" s="2"/>
     </row>
     <row r="297" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3673,44 +3684,44 @@
       <c r="T302" s="2"/>
     </row>
     <row r="303" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D303" s="5"/>
       <c r="T303" s="2"/>
     </row>
     <row r="304" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D304" s="5"/>
       <c r="T304" s="2"/>
     </row>
     <row r="305" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C305" s="5"/>
       <c r="T305" s="2"/>
     </row>
     <row r="306" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C306" s="5"/>
       <c r="T306" s="2"/>
     </row>
     <row r="307" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="T307" s="2"/>
     </row>
     <row r="308" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D308" s="5"/>
       <c r="T308" s="2"/>
     </row>
     <row r="309" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D309" s="5"/>
       <c r="T309" s="2"/>
     </row>
     <row r="310" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="T310" s="2"/>
     </row>
     <row r="311" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D311" s="5"/>
       <c r="T311" s="2"/>
     </row>
     <row r="312" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D312" s="5"/>
       <c r="T312" s="2"/>
     </row>
     <row r="313" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C313" s="5"/>
       <c r="T313" s="2"/>
     </row>
     <row r="314" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C314" s="5"/>
       <c r="T314" s="2"/>
     </row>
     <row r="315" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3720,18 +3731,17 @@
       <c r="T316" s="2"/>
     </row>
     <row r="317" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D317" s="5"/>
       <c r="T317" s="2"/>
     </row>
     <row r="318" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D318" s="5"/>
       <c r="T318" s="2"/>
     </row>
     <row r="319" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D319" s="5"/>
       <c r="T319" s="2"/>
     </row>
     <row r="320" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C320" s="5"/>
+      <c r="D320" s="5"/>
       <c r="T320" s="2"/>
     </row>
     <row r="321" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3739,41 +3749,42 @@
       <c r="T321" s="2"/>
     </row>
     <row r="322" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C322" s="5"/>
       <c r="T322" s="2"/>
     </row>
     <row r="323" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D323" s="5"/>
       <c r="T323" s="2"/>
     </row>
     <row r="324" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D324" s="5"/>
       <c r="T324" s="2"/>
     </row>
     <row r="325" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D325" s="5"/>
       <c r="T325" s="2"/>
     </row>
     <row r="326" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D326" s="5"/>
       <c r="T326" s="2"/>
     </row>
     <row r="327" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C327" s="5"/>
       <c r="T327" s="2"/>
     </row>
     <row r="328" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C328" s="5"/>
       <c r="T328" s="2"/>
     </row>
     <row r="329" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C329" s="5"/>
       <c r="T329" s="2"/>
     </row>
     <row r="330" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C330" s="5"/>
       <c r="T330" s="2"/>
     </row>
     <row r="331" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D331" s="5"/>
       <c r="T331" s="2"/>
     </row>
     <row r="332" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D332" s="5"/>
       <c r="T332" s="2"/>
     </row>
     <row r="333" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3786,20 +3797,20 @@
       <c r="T335" s="2"/>
     </row>
     <row r="336" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C336" s="5"/>
       <c r="T336" s="2"/>
     </row>
     <row r="337" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C337" s="5"/>
       <c r="T337" s="2"/>
     </row>
     <row r="338" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="T338" s="2"/>
     </row>
     <row r="339" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D339" s="5"/>
       <c r="T339" s="2"/>
     </row>
     <row r="340" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D340" s="5"/>
       <c r="T340" s="2"/>
     </row>
     <row r="341" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3821,10 +3832,10 @@
       <c r="T346" s="2"/>
     </row>
     <row r="347" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D347" s="5"/>
       <c r="T347" s="2"/>
     </row>
     <row r="348" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D348" s="5"/>
       <c r="T348" s="2"/>
     </row>
     <row r="349" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3870,10 +3881,10 @@
       <c r="T362" s="2"/>
     </row>
     <row r="363" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C363" s="5"/>
       <c r="T363" s="2"/>
     </row>
     <row r="364" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C364" s="5"/>
       <c r="T364" s="2"/>
     </row>
     <row r="365" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3883,10 +3894,10 @@
       <c r="T366" s="2"/>
     </row>
     <row r="367" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D367" s="5"/>
       <c r="T367" s="2"/>
     </row>
     <row r="368" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D368" s="5"/>
       <c r="T368" s="2"/>
     </row>
     <row r="369" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3896,17 +3907,17 @@
       <c r="T370" s="2"/>
     </row>
     <row r="371" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D371" s="5"/>
       <c r="T371" s="2"/>
     </row>
     <row r="372" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D372" s="5"/>
       <c r="T372" s="2"/>
     </row>
     <row r="373" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D373" s="5"/>
       <c r="T373" s="2"/>
     </row>
     <row r="374" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D374" s="5"/>
       <c r="T374" s="2"/>
     </row>
     <row r="375" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3916,20 +3927,20 @@
       <c r="T376" s="2"/>
     </row>
     <row r="377" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D377" s="5"/>
       <c r="T377" s="2"/>
     </row>
     <row r="378" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D378" s="5"/>
       <c r="T378" s="2"/>
     </row>
     <row r="379" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="T379" s="2"/>
     </row>
     <row r="380" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D380" s="5"/>
       <c r="T380" s="2"/>
     </row>
     <row r="381" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D381" s="5"/>
       <c r="T381" s="2"/>
     </row>
     <row r="382" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3942,13 +3953,13 @@
       <c r="T384" s="2"/>
     </row>
     <row r="385" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G385" s="1" t="s">
-        <v>288</v>
-      </c>
-      <c r="H385" s="5"/>
       <c r="T385" s="2"/>
     </row>
     <row r="386" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G386" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="H386" s="5"/>
       <c r="T386" s="2"/>
     </row>
     <row r="387" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3961,10 +3972,10 @@
       <c r="T389" s="2"/>
     </row>
     <row r="390" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F390" s="5"/>
       <c r="T390" s="2"/>
     </row>
     <row r="391" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F391" s="5"/>
       <c r="T391" s="2"/>
     </row>
     <row r="392" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3977,17 +3988,17 @@
       <c r="T394" s="2"/>
     </row>
     <row r="395" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D395" s="5"/>
       <c r="T395" s="2"/>
     </row>
     <row r="396" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D396" s="5"/>
       <c r="T396" s="2"/>
     </row>
     <row r="397" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C397" s="5"/>
       <c r="T397" s="2"/>
     </row>
     <row r="398" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C398" s="5"/>
       <c r="T398" s="2"/>
     </row>
     <row r="399" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4000,10 +4011,10 @@
       <c r="T401" s="2"/>
     </row>
     <row r="402" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C402" s="5"/>
       <c r="T402" s="2"/>
     </row>
     <row r="403" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C403" s="5"/>
       <c r="T403" s="2"/>
     </row>
     <row r="404" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4016,10 +4027,10 @@
       <c r="T406" s="2"/>
     </row>
     <row r="407" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F407" s="5"/>
       <c r="T407" s="2"/>
     </row>
     <row r="408" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F408" s="5"/>
       <c r="T408" s="2"/>
     </row>
     <row r="409" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4034,7 +4045,9 @@
     <row r="412" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="T412" s="2"/>
     </row>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="413" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="T413" s="2"/>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>